<commit_message>
formatting update for percent column
</commit_message>
<xml_diff>
--- a/arcgis pro/excel-summary/Excel_Test_File.xlsx
+++ b/arcgis pro/excel-summary/Excel_Test_File.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestData" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -46,8 +47,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -729,4 +731,140 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(TestData!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(TestData!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(TestData!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>COUNTA(TestData!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new data sources
</commit_message>
<xml_diff>
--- a/arcgis pro/excel-summary/Excel_Test_File.xlsx
+++ b/arcgis pro/excel-summary/Excel_Test_File.xlsx
@@ -57,6 +57,14 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_47" sheetId="49" state="visible" r:id="rId49"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_48" sheetId="50" state="visible" r:id="rId50"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_49" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_50" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_51" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_52" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_53" sheetId="55" state="visible" r:id="rId55"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_54" sheetId="56" state="visible" r:id="rId56"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_55" sheetId="57" state="visible" r:id="rId57"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_56" sheetId="58" state="visible" r:id="rId58"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_57" sheetId="59" state="visible" r:id="rId59"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -6050,6 +6058,922 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(TestData!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(TestData!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(TestData!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>COUNTA(TestData!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(TestData!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(TestData!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(TestData!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>COUNTA(TestData!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7">
+        <f>COUNTA(TestData!F:F)-1</f>
+        <v/>
+      </c>
+      <c r="C7">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D7" s="1">
+        <f>B7/C7</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(Summary_1!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(Summary_1!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(Summary_1!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6">
+        <f>COUNTA(Summary_1!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(TestData!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(TestData!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(TestData!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>COUNTA(TestData!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(TestData!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(TestData!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(TestData!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>COUNTA(TestData!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7">
+        <f>COUNTA(TestData!F:F)-1</f>
+        <v/>
+      </c>
+      <c r="C7">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D7" s="1">
+        <f>B7/C7</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(Summary_1!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(Summary_1!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(Summary_1!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6">
+        <f>COUNTA(Summary_1!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
fix excel sheets and improve UI
</commit_message>
<xml_diff>
--- a/arcgis pro/excel-summary/Excel_Test_File.xlsx
+++ b/arcgis pro/excel-summary/Excel_Test_File.xlsx
@@ -65,6 +65,12 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_55" sheetId="57" state="visible" r:id="rId57"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_56" sheetId="58" state="visible" r:id="rId58"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_57" sheetId="59" state="visible" r:id="rId59"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_58" sheetId="60" state="visible" r:id="rId60"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_59" sheetId="61" state="visible" r:id="rId61"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_60" sheetId="62" state="visible" r:id="rId62"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_61" sheetId="63" state="visible" r:id="rId63"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_62" sheetId="64" state="visible" r:id="rId64"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary_63" sheetId="65" state="visible" r:id="rId65"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1856,7 +1862,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7110,6 +7116,641 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(TestData!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(TestData!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(TestData!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>COUNTA(TestData!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(TestData!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(TestData!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(TestData!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>COUNTA(TestData!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7">
+        <f>COUNTA(TestData!F:F)-1</f>
+        <v/>
+      </c>
+      <c r="C7">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D7" s="1">
+        <f>B7/C7</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(Summary_1!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(Summary_1!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(Summary_1!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6">
+        <f>COUNTA(Summary_1!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(Summary_1!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D2" s="1">
+        <f>B2/C2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>COUNTA(TestData!B:B)-1</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f>B3/C3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="B4">
+        <f>COUNTA(TestData!C:C)-1</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D4" s="1">
+        <f>B4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTA(TestData!D:D)-1</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D5" s="1">
+        <f>B5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="B6">
+        <f>COUNTA(TestData!E:E)-1</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>COUNTA(TestData!A:A)-1</f>
+        <v/>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Column Heading</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>